<commit_message>
added making a copy of the excel file function.
</commit_message>
<xml_diff>
--- a/src/test/resources/ER.xlsx
+++ b/src/test/resources/ER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdroh\IdeaProjects\SauceDemoTest\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FFB2B4-872D-4263-B53C-778FD6B048BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB72819D-6800-4B5B-9D79-033360007B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Price Total Before Tax</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Total After Tax</t>
   </si>
@@ -58,6 +55,12 @@
   </si>
   <si>
     <t>Tax Amount</t>
+  </si>
+  <si>
+    <t>Total Amount round upto 2 decimal</t>
+  </si>
+  <si>
+    <t>Total Price Before Tax</t>
   </si>
 </sst>
 </file>
@@ -240,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -252,6 +255,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -548,30 +554,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="31.5546875" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="18.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="12"/>
+      <c r="A1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="n">
-        <v>29.99</v>
+        <v>113.95</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.35">
@@ -583,58 +589,75 @@
       <c r="B4" s="9"/>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="14"/>
+      <c r="A5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="n">
-        <f>B10</f>
-        <v>2.4</v>
+        <f>B12</f>
+        <v>9.12</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <f>B13</f>
+        <v>123.07</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+    </row>
+    <row r="9" spans="1:2" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="3" t="n">
-        <f>B2+B6</f>
-        <v>32.39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="B10" s="18"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="15"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="B11" s="6" t="n">
+        <f>(B2*8)/100</f>
+        <v>9.116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="6" t="n">
-        <f>(B2*8)/100</f>
-        <v>2.3992</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="5" t="n">
-        <f>ROUND(B9,2)</f>
-        <v>2.4</v>
+      <c r="B12" s="5" t="n">
+        <f>ROUND(B11,2)</f>
+        <v>9.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="11" t="n">
+        <f>ROUND(B2+B12,2)</f>
+        <v>123.07</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>